<commit_message>
Deploying to gh-pages from  @ 34851be926b266cf415dc528bf51f0a75be94f47 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Национальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Национальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -184,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +266,33 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -342,7 +369,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,6 +425,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8154,9 +8186,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -8165,7 +8199,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="24" customHeight="1">
+    <row r="1" spans="1:14" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
@@ -8176,7 +8210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.5" customHeight="1">
+    <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -8187,7 +8221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75" thickBot="1">
+    <row r="3" spans="1:14" ht="12.75" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8198,8 +8232,9 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
+      <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8239,8 +8274,11 @@
       <c r="M4" s="12">
         <v>2019</v>
       </c>
+      <c r="N4" s="19">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -8280,8 +8318,11 @@
       <c r="M5" s="14">
         <v>0.54933623931578479</v>
       </c>
+      <c r="N5" s="20">
+        <v>0.89148765717852163</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
         <v>24</v>
       </c>
@@ -8321,8 +8362,11 @@
       <c r="M6" s="15">
         <v>0.1</v>
       </c>
+      <c r="N6" s="21">
+        <v>0.31407178438278893</v>
+      </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -8362,8 +8406,11 @@
       <c r="M7" s="15">
         <v>0.8</v>
       </c>
+      <c r="N7" s="21">
+        <v>1.220561325080239</v>
+      </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
         <v>28</v>
       </c>
@@ -8403,8 +8450,11 @@
       <c r="M8" s="15">
         <v>0.3392671909690585</v>
       </c>
+      <c r="N8" s="22">
+        <v>1.6290305205827647</v>
+      </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -8444,8 +8494,11 @@
       <c r="M9" s="15">
         <v>0.56205045247263075</v>
       </c>
+      <c r="N9" s="22">
+        <v>1.4841131607226035</v>
+      </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
         <v>32</v>
       </c>
@@ -8485,8 +8538,11 @@
       <c r="M10" s="15">
         <v>1.2604968981368243</v>
       </c>
+      <c r="N10" s="22">
+        <v>0.43494800834006392</v>
+      </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
@@ -8526,8 +8582,11 @@
       <c r="M11" s="15">
         <v>2.4816289901846873</v>
       </c>
+      <c r="N11" s="22">
+        <v>4.5037215639801795</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1">
+    <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -8567,8 +8626,11 @@
       <c r="M12" s="15">
         <v>0.88079865305212723</v>
       </c>
+      <c r="N12" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -8608,8 +8670,11 @@
       <c r="M13" s="15">
         <v>0</v>
       </c>
+      <c r="N13" s="22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>40</v>
       </c>
@@ -8649,8 +8714,11 @@
       <c r="M14" s="15">
         <v>0.16260204281171109</v>
       </c>
+      <c r="N14" s="22">
+        <v>1.3481169038547842</v>
+      </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -8690,8 +8758,11 @@
       <c r="M15" s="15">
         <v>0</v>
       </c>
+      <c r="N15" s="22">
+        <v>0.28229127286371936</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" ht="12.75" thickBot="1">
+    <row r="16" spans="1:14" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>44</v>
       </c>
@@ -8729,6 +8800,9 @@
         <v>0.55610781362635098</v>
       </c>
       <c r="M16" s="17">
+        <v>0</v>
+      </c>
+      <c r="N16" s="23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 8b4f3478c1efe3c3e12d23e77b5223b88a73f69d 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -39,12 +39,6 @@
     <t>Items</t>
   </si>
   <si>
-    <t>город</t>
-  </si>
-  <si>
-    <t>село</t>
-  </si>
-  <si>
     <t>1.1.1.1a Уровень крайней бедности</t>
   </si>
   <si>
@@ -81,12 +75,6 @@
     <t>Kyrgyz Republic</t>
   </si>
   <si>
-    <t>urban</t>
-  </si>
-  <si>
-    <t>rural</t>
-  </si>
-  <si>
     <t>…</t>
   </si>
   <si>
@@ -100,12 +88,6 @@
   </si>
   <si>
     <t>(жалпы санына каратапайыз менен)</t>
-  </si>
-  <si>
-    <t>шаар</t>
-  </si>
-  <si>
-    <t>айыл</t>
   </si>
   <si>
     <t>Кыргыз Республикасы</t>
@@ -175,6 +157,24 @@
   </si>
   <si>
     <t>*2013ж. чейин Ош ш. кошо алганда</t>
+  </si>
+  <si>
+    <t>Шаар жерлери</t>
+  </si>
+  <si>
+    <t>Городские поселения</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Айыл аймагы</t>
+  </si>
+  <si>
+    <t>Сельская местность</t>
+  </si>
+  <si>
+    <t>Village</t>
   </si>
 </sst>
 </file>
@@ -8188,8 +8188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -8201,24 +8201,24 @@
   <sheetData>
     <row r="1" spans="1:14" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.75" thickBot="1">
@@ -8280,13 +8280,13 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="14">
         <v>5.3438169958924879</v>
@@ -8324,13 +8324,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D6" s="15">
         <v>4.2168631530813512</v>
@@ -8368,13 +8368,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D7" s="15">
         <v>5.9930922559799589</v>
@@ -8412,13 +8412,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D8" s="15">
         <v>5.1808804816231708</v>
@@ -8456,13 +8456,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D9" s="15">
         <v>6.4380322738993074</v>
@@ -8500,13 +8500,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" s="15">
         <v>2.4787267316625954</v>
@@ -8544,13 +8544,13 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="15">
         <v>12.036462028653192</v>
@@ -8588,13 +8588,13 @@
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" s="15">
         <v>8.3331494569001308</v>
@@ -8632,13 +8632,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="15">
         <v>5.0122940777216947</v>
@@ -8676,13 +8676,13 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" s="15">
         <v>3.5353129806100583</v>
@@ -8720,13 +8720,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D15" s="15">
         <v>0.53092532677015958</v>
@@ -8764,22 +8764,22 @@
     </row>
     <row r="16" spans="1:14" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G16" s="17">
         <v>3.5070632421313164</v>
@@ -8808,13 +8808,13 @@
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ d92d6b6bb39af5aaf864c7d0208038fbc61582e0 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -87,9 +87,6 @@
     <t>1.1.1.1а Деңгээли өтө жакырчылык калк</t>
   </si>
   <si>
-    <t>(жалпы санына каратапайыз менен)</t>
-  </si>
-  <si>
     <t>Кыргыз Республикасы</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Village</t>
+  </si>
+  <si>
+    <t>(жалпы калктын санына карата пайыз менен)</t>
   </si>
 </sst>
 </file>
@@ -8189,7 +8189,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -8212,7 +8212,7 @@
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -8280,7 +8280,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -8324,13 +8324,13 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="D6" s="15">
         <v>4.2168631530813512</v>
@@ -8368,13 +8368,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="D7" s="15">
         <v>5.9930922559799589</v>
@@ -8412,13 +8412,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="15">
         <v>5.1808804816231708</v>
@@ -8456,13 +8456,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="15">
         <v>6.4380322738993074</v>
@@ -8500,13 +8500,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="15">
         <v>2.4787267316625954</v>
@@ -8544,13 +8544,13 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="15">
         <v>12.036462028653192</v>
@@ -8588,13 +8588,13 @@
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="15">
         <v>8.3331494569001308</v>
@@ -8632,13 +8632,13 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15">
         <v>5.0122940777216947</v>
@@ -8676,13 +8676,13 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="15">
         <v>3.5353129806100583</v>
@@ -8720,13 +8720,13 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="15">
         <v>0.53092532677015958</v>
@@ -8764,13 +8764,13 @@
     </row>
     <row r="16" spans="1:14" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>15</v>
@@ -8808,13 +8808,13 @@
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ d7261741d34ceb6a6ebf91ec8ade3ac4f7b42eaa 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -184,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +293,25 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman CE"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman CE"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -369,7 +388,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,6 +449,10 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8186,11 +8209,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -8199,7 +8220,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" customHeight="1">
+    <row r="1" spans="1:15" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -8210,7 +8231,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13.5" customHeight="1">
+    <row r="2" spans="1:15" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -8221,7 +8242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="12.75" thickBot="1">
+    <row r="3" spans="1:15" ht="12.75" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8233,8 +8254,9 @@
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:15" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8277,8 +8299,11 @@
       <c r="N4" s="19">
         <v>2020</v>
       </c>
+      <c r="O4" s="24">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15" ht="12.75">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -8321,8 +8346,11 @@
       <c r="N5" s="20">
         <v>0.89148765717852163</v>
       </c>
+      <c r="O5" s="25">
+        <v>6.0337796775071091</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15" ht="12.75">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -8365,8 +8393,11 @@
       <c r="N6" s="21">
         <v>0.31407178438278893</v>
       </c>
+      <c r="O6" s="26">
+        <v>7.3075058743442511</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15" ht="12.75">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -8409,8 +8440,11 @@
       <c r="N7" s="21">
         <v>1.220561325080239</v>
       </c>
+      <c r="O7" s="26">
+        <v>5.2767607763499562</v>
+      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15" ht="12.75">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -8453,8 +8487,11 @@
       <c r="N8" s="22">
         <v>1.6290305205827647</v>
       </c>
+      <c r="O8" s="26">
+        <v>10.064200140319592</v>
+      </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15" ht="12.75">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -8497,8 +8534,11 @@
       <c r="N9" s="22">
         <v>1.4841131607226035</v>
       </c>
+      <c r="O9" s="26">
+        <v>7.5445007460298559</v>
+      </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15" ht="12.75">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -8541,8 +8581,11 @@
       <c r="N10" s="22">
         <v>0.43494800834006392</v>
       </c>
+      <c r="O10" s="26">
+        <v>7.9562092224762884</v>
+      </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15" ht="12.75">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -8585,8 +8628,11 @@
       <c r="N11" s="22">
         <v>4.5037215639801795</v>
       </c>
+      <c r="O11" s="26">
+        <v>8.1696953402867685</v>
+      </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1">
+    <row r="12" spans="1:15" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -8629,8 +8675,11 @@
       <c r="N12" s="22">
         <v>0</v>
       </c>
+      <c r="O12" s="26">
+        <v>2.0701729813092102</v>
+      </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15" ht="12.75">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -8673,8 +8722,11 @@
       <c r="N13" s="22">
         <v>0</v>
       </c>
+      <c r="O13" s="26">
+        <v>2.6482523478927704</v>
+      </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15" ht="12.75">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -8717,8 +8769,11 @@
       <c r="N14" s="22">
         <v>1.3481169038547842</v>
       </c>
+      <c r="O14" s="26">
+        <v>3.9561647100749857</v>
+      </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15" ht="12.75">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -8761,8 +8816,11 @@
       <c r="N15" s="22">
         <v>0.28229127286371936</v>
       </c>
+      <c r="O15" s="26">
+        <v>9.4645167179465837</v>
+      </c>
     </row>
-    <row r="16" spans="1:14" ht="12.75" thickBot="1">
+    <row r="16" spans="1:15" ht="13.5" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -8804,6 +8862,9 @@
       </c>
       <c r="N16" s="23">
         <v>0</v>
+      </c>
+      <c r="O16" s="27">
+        <v>3.1019579996103404</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 4315f606f30ae9a2dbda139bcee951adab3b430f 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -184,7 +184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,23 +294,9 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Times New Roman CE"/>
-      <family val="1"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="9"/>
       <name val="Times New Roman CE"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman CE"/>
-      <family val="1"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,7 +374,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,10 +435,11 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8209,9 +8196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -8220,7 +8209,7 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" customHeight="1">
+    <row r="1" spans="1:16" ht="24" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>18</v>
       </c>
@@ -8231,7 +8220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13.5" customHeight="1">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -8242,7 +8231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="12.75" thickBot="1">
+    <row r="3" spans="1:16" ht="12.75" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8255,8 +8244,9 @@
       <c r="M3" s="11"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8299,11 +8289,14 @@
       <c r="N4" s="19">
         <v>2020</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="19">
         <v>2021</v>
       </c>
+      <c r="P4" s="28">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" ht="12.75">
+    <row r="5" spans="1:16">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -8346,11 +8339,14 @@
       <c r="N5" s="20">
         <v>0.89148765717852163</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="20">
         <v>6.0337796775071091</v>
       </c>
+      <c r="P5" s="24">
+        <v>5.9676405075953687</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="12.75">
+    <row r="6" spans="1:16">
       <c r="A6" s="7" t="s">
         <v>42</v>
       </c>
@@ -8393,11 +8389,14 @@
       <c r="N6" s="21">
         <v>0.31407178438278893</v>
       </c>
-      <c r="O6" s="26">
+      <c r="O6" s="25">
         <v>7.3075058743442511</v>
       </c>
+      <c r="P6" s="26">
+        <v>5.6044335798150424</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="12.75">
+    <row r="7" spans="1:16">
       <c r="A7" s="8" t="s">
         <v>45</v>
       </c>
@@ -8440,11 +8439,14 @@
       <c r="N7" s="21">
         <v>1.220561325080239</v>
       </c>
-      <c r="O7" s="26">
+      <c r="O7" s="25">
         <v>5.2767607763499562</v>
       </c>
+      <c r="P7" s="26">
+        <v>6.1789553077823856</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" ht="12.75">
+    <row r="8" spans="1:16">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
@@ -8487,11 +8489,14 @@
       <c r="N8" s="22">
         <v>1.6290305205827647</v>
       </c>
-      <c r="O8" s="26">
+      <c r="O8" s="25">
         <v>10.064200140319592</v>
       </c>
+      <c r="P8" s="26">
+        <v>16.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" ht="12.75">
+    <row r="9" spans="1:16">
       <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
@@ -8534,11 +8539,14 @@
       <c r="N9" s="22">
         <v>1.4841131607226035</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="25">
         <v>7.5445007460298559</v>
       </c>
+      <c r="P9" s="26">
+        <v>9.1</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" ht="12.75">
+    <row r="10" spans="1:16">
       <c r="A10" s="9" t="s">
         <v>25</v>
       </c>
@@ -8581,11 +8589,14 @@
       <c r="N10" s="22">
         <v>0.43494800834006392</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="25">
         <v>7.9562092224762884</v>
       </c>
+      <c r="P10" s="26">
+        <v>8.8000000000000007</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" ht="12.75">
+    <row r="11" spans="1:16">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
@@ -8628,11 +8639,14 @@
       <c r="N11" s="22">
         <v>4.5037215639801795</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="25">
         <v>8.1696953402867685</v>
       </c>
+      <c r="P11" s="26">
+        <v>6.7</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1">
+    <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -8675,11 +8689,14 @@
       <c r="N12" s="22">
         <v>0</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="25">
         <v>2.0701729813092102</v>
       </c>
+      <c r="P12" s="26">
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" ht="12.75">
+    <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -8722,11 +8739,14 @@
       <c r="N13" s="22">
         <v>0</v>
       </c>
-      <c r="O13" s="26">
+      <c r="O13" s="25">
         <v>2.6482523478927704</v>
       </c>
+      <c r="P13" s="26">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
-    <row r="14" spans="1:15" ht="12.75">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -8769,11 +8789,14 @@
       <c r="N14" s="22">
         <v>1.3481169038547842</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="25">
         <v>3.9561647100749857</v>
       </c>
+      <c r="P14" s="26">
+        <v>5.0999999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" ht="12.75">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -8816,11 +8839,14 @@
       <c r="N15" s="22">
         <v>0.28229127286371936</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O15" s="25">
         <v>9.4645167179465837</v>
       </c>
+      <c r="P15" s="26">
+        <v>3.9</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" ht="13.5" thickBot="1">
+    <row r="16" spans="1:16" ht="12.75" thickBot="1">
       <c r="A16" s="10" t="s">
         <v>37</v>
       </c>
@@ -8865,6 +8891,9 @@
       </c>
       <c r="O16" s="27">
         <v>3.1019579996103404</v>
+      </c>
+      <c r="P16" s="27">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1">

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ ec3cb725c8f060ad398b3a92b5e83e1369047b93 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.1.1.1a.xlsx
+++ b/en/downloads/data-excel/1.1.1.1a.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Kyrgyz Republic</t>
-  </si>
-  <si>
-    <t>…</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.1.1a Level of extreme poverty </t>
@@ -176,6 +173,54 @@
   <si>
     <t>(жалпы калктын санына карата пайыз менен)</t>
   </si>
+  <si>
+    <t>По полу</t>
+  </si>
+  <si>
+    <t>Место проживания</t>
+  </si>
+  <si>
+    <t>Женщины</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Мужчины</t>
+  </si>
+  <si>
+    <t>Жынысы боюнча</t>
+  </si>
+  <si>
+    <t>Аялдар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Эркектер </t>
+  </si>
+  <si>
+    <t>by sex</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>Urbanisation</t>
+  </si>
+  <si>
+    <t>Жашаган жери</t>
+  </si>
+  <si>
+    <t>Аймактар боюнча</t>
+  </si>
+  <si>
+    <t>По территории</t>
+  </si>
+  <si>
+    <t>By territory</t>
+  </si>
 </sst>
 </file>
 
@@ -184,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +343,19 @@
       <name val="Times New Roman CE"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -374,7 +432,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -412,9 +470,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -435,11 +490,26 @@
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8196,11 +8266,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
@@ -8209,29 +8277,29 @@
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="24" customHeight="1">
-      <c r="A1" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:17" ht="24" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>16</v>
+      <c r="C1" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13.5" customHeight="1">
+    <row r="2" spans="1:17" ht="13.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="12.75" thickBot="1">
+    <row r="3" spans="1:17" ht="13.5" customHeight="1" thickBot="1">
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8245,8 +8313,9 @@
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:17" ht="14.25" customHeight="1" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -8286,625 +8355,839 @@
       <c r="M4" s="12">
         <v>2019</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="18">
         <v>2020</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="18">
         <v>2021</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="18">
         <v>2022</v>
       </c>
+      <c r="Q4" s="18">
+        <v>2023</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" ht="14.25" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>5.3438169958924879</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>4.545728690156194</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>4.3902104224137357</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>2.7520531699173962</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>1.2045438763134317</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
         <v>1.2463</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>0.79950533734625018</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <v>0.75126418709986076</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>0.55684909247351222</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <v>0.54933623931578479</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="19">
         <v>0.89148765717852163</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="19">
         <v>6.0337796775071091</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="19">
         <v>5.9676405075953687</v>
       </c>
+      <c r="Q5" s="19">
+        <v>4.9547183120610843</v>
+      </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:17" s="28" customFormat="1" ht="15">
+      <c r="A6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+    </row>
+    <row r="7" spans="1:17" s="28" customFormat="1" ht="15">
+      <c r="A7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0.68519413875264201</v>
+      </c>
+      <c r="L7" s="27">
+        <v>0.52778295592322599</v>
+      </c>
+      <c r="M7" s="27">
+        <v>0.55180198070156894</v>
+      </c>
+      <c r="N7" s="27">
+        <v>0.80960724343075641</v>
+      </c>
+      <c r="O7" s="27">
+        <v>6.2123810703447084</v>
+      </c>
+      <c r="P7" s="27">
+        <v>6.2</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>4.9263803296199171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="28" customFormat="1" ht="15">
+      <c r="A8" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0.82404503217287961</v>
+      </c>
+      <c r="L8" s="27">
+        <v>0.589459031995476</v>
+      </c>
+      <c r="M8" s="27">
+        <v>0.54655576288689411</v>
+      </c>
+      <c r="N8" s="27">
+        <v>0.98245128998233044</v>
+      </c>
+      <c r="O8" s="27">
+        <v>5.8348173264224643</v>
+      </c>
+      <c r="P8" s="27">
+        <v>5.7</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>4.9857836040976133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" s="28" customFormat="1" ht="15">
+      <c r="A9" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+    </row>
+    <row r="10" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D10" s="14">
+        <v>4.2168631530813512</v>
+      </c>
+      <c r="E10" s="14">
+        <v>2.5713927856479444</v>
+      </c>
+      <c r="F10" s="14">
+        <v>4.2453039507137298</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1.622592666205378</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1.3352534216041274</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1.0364</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.32993924401723507</v>
+      </c>
+      <c r="K10" s="14">
+        <v>0.31702172210916746</v>
+      </c>
+      <c r="L10" s="14">
+        <v>0.2403586586679928</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="N10" s="20">
+        <v>0.31407178438278893</v>
+      </c>
+      <c r="O10" s="23">
+        <v>7.3075058743442511</v>
+      </c>
+      <c r="P10" s="23">
+        <v>5.6044335798150424</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>5.2409183200762754</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="15">
-        <v>4.2168631530813512</v>
-      </c>
-      <c r="E6" s="15">
-        <v>2.5713927856479444</v>
-      </c>
-      <c r="F6" s="15">
-        <v>4.2453039507137298</v>
-      </c>
-      <c r="G6" s="15">
-        <v>1.622592666205378</v>
-      </c>
-      <c r="H6" s="15">
-        <v>1.3352534216041274</v>
-      </c>
-      <c r="I6" s="15">
-        <v>1.0364</v>
-      </c>
-      <c r="J6" s="15">
-        <v>0.32993924401723507</v>
-      </c>
-      <c r="K6" s="15">
-        <v>0.31702172210916746</v>
-      </c>
-      <c r="L6" s="15">
-        <v>0.2403586586679928</v>
-      </c>
-      <c r="M6" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="N6" s="21">
-        <v>0.31407178438278893</v>
-      </c>
-      <c r="O6" s="25">
-        <v>7.3075058743442511</v>
-      </c>
-      <c r="P6" s="26">
-        <v>5.6044335798150424</v>
+      <c r="B11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14">
+        <v>5.9930922559799589</v>
+      </c>
+      <c r="E11" s="14">
+        <v>5.7195315396021638</v>
+      </c>
+      <c r="F11" s="14">
+        <v>4.474039629820532</v>
+      </c>
+      <c r="G11" s="14">
+        <v>3.3387697541408841</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1.1307049829892899</v>
+      </c>
+      <c r="I11" s="14">
+        <v>1.3613</v>
+      </c>
+      <c r="J11" s="14">
+        <v>1.0572316812127296</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0.9904939556603013</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0.7328783431070176</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="N11" s="20">
+        <v>1.220561325080239</v>
+      </c>
+      <c r="O11" s="23">
+        <v>5.2767607763499562</v>
+      </c>
+      <c r="P11" s="23">
+        <v>6.1789553077823856</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>4.7888452943619573</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="15">
-        <v>5.9930922559799589</v>
-      </c>
-      <c r="E7" s="15">
-        <v>5.7195315396021638</v>
-      </c>
-      <c r="F7" s="15">
-        <v>4.474039629820532</v>
-      </c>
-      <c r="G7" s="15">
-        <v>3.3387697541408841</v>
-      </c>
-      <c r="H7" s="15">
-        <v>1.1307049829892899</v>
-      </c>
-      <c r="I7" s="15">
-        <v>1.3613</v>
-      </c>
-      <c r="J7" s="15">
-        <v>1.0572316812127296</v>
-      </c>
-      <c r="K7" s="15">
-        <v>0.9904939556603013</v>
-      </c>
-      <c r="L7" s="15">
-        <v>0.7328783431070176</v>
-      </c>
-      <c r="M7" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="N7" s="21">
-        <v>1.220561325080239</v>
-      </c>
-      <c r="O7" s="25">
-        <v>5.2767607763499562</v>
-      </c>
-      <c r="P7" s="26">
-        <v>6.1789553077823856</v>
-      </c>
+    <row r="12" spans="1:17" customFormat="1" ht="15">
+      <c r="A12" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="9" t="s">
+    <row r="13" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D13" s="14">
+        <v>5.1808804816231708</v>
+      </c>
+      <c r="E13" s="14">
+        <v>3.5712525519800784</v>
+      </c>
+      <c r="F13" s="14">
+        <v>2.4298219022359215</v>
+      </c>
+      <c r="G13" s="14">
+        <v>7.9920581957878776</v>
+      </c>
+      <c r="H13" s="14">
+        <v>2.6473978814209165</v>
+      </c>
+      <c r="I13" s="14">
+        <v>4.0069999999999997</v>
+      </c>
+      <c r="J13" s="14">
+        <v>0.32112435111554388</v>
+      </c>
+      <c r="K13" s="14">
+        <v>3.3941360063781501</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0.87300583877555049</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0.3392671909690585</v>
+      </c>
+      <c r="N13" s="21">
+        <v>1.6290305205827647</v>
+      </c>
+      <c r="O13" s="23">
+        <v>10.064200140319592</v>
+      </c>
+      <c r="P13" s="23">
+        <v>16.5</v>
+      </c>
+      <c r="Q13" s="23">
+        <v>16.145310230913825</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="15">
-        <v>5.1808804816231708</v>
-      </c>
-      <c r="E8" s="15">
-        <v>3.5712525519800784</v>
-      </c>
-      <c r="F8" s="15">
-        <v>2.4298219022359215</v>
-      </c>
-      <c r="G8" s="15">
-        <v>7.9920581957878776</v>
-      </c>
-      <c r="H8" s="15">
-        <v>2.6473978814209165</v>
-      </c>
-      <c r="I8" s="15">
-        <v>4.0069999999999997</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0.32112435111554388</v>
-      </c>
-      <c r="K8" s="15">
-        <v>3.3941360063781501</v>
-      </c>
-      <c r="L8" s="15">
-        <v>0.87300583877555049</v>
-      </c>
-      <c r="M8" s="15">
-        <v>0.3392671909690585</v>
-      </c>
-      <c r="N8" s="22">
-        <v>1.6290305205827647</v>
-      </c>
-      <c r="O8" s="25">
-        <v>10.064200140319592</v>
-      </c>
-      <c r="P8" s="26">
-        <v>16.5</v>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="14">
+        <v>6.4380322738993074</v>
+      </c>
+      <c r="E14" s="14">
+        <v>6.6554187654394825</v>
+      </c>
+      <c r="F14" s="14">
+        <v>14.126082809346473</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1.4181571804450666</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1.06205582454581</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0.47739999999999999</v>
+      </c>
+      <c r="J14" s="14">
+        <v>0.11107551172966013</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <v>1.011691375024679</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0.56205045247263075</v>
+      </c>
+      <c r="N14" s="21">
+        <v>1.4841131607226035</v>
+      </c>
+      <c r="O14" s="23">
+        <v>7.5445007460298559</v>
+      </c>
+      <c r="P14" s="23">
+        <v>9.1</v>
+      </c>
+      <c r="Q14" s="23">
+        <v>5.0414052649559933</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="9" t="s">
+    <row r="15" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="15">
-        <v>6.4380322738993074</v>
-      </c>
-      <c r="E9" s="15">
-        <v>6.6554187654394825</v>
-      </c>
-      <c r="F9" s="15">
-        <v>14.126082809346473</v>
-      </c>
-      <c r="G9" s="15">
-        <v>1.4181571804450666</v>
-      </c>
-      <c r="H9" s="15">
-        <v>1.06205582454581</v>
-      </c>
-      <c r="I9" s="15">
-        <v>0.47739999999999999</v>
-      </c>
-      <c r="J9" s="15">
-        <v>0.11107551172966013</v>
-      </c>
-      <c r="K9" s="15">
+      <c r="B15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="14">
+        <v>2.4787267316625954</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1.5072935699864518</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0.13114731930321041</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1.9058703261018888</v>
+      </c>
+      <c r="H15" s="14">
         <v>0</v>
       </c>
-      <c r="L9" s="15">
-        <v>1.011691375024679</v>
-      </c>
-      <c r="M9" s="15">
-        <v>0.56205045247263075</v>
-      </c>
-      <c r="N9" s="22">
-        <v>1.4841131607226035</v>
-      </c>
-      <c r="O9" s="25">
-        <v>7.5445007460298559</v>
-      </c>
-      <c r="P9" s="26">
-        <v>9.1</v>
+      <c r="I15" s="14">
+        <v>0.41110000000000002</v>
+      </c>
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <v>1.0368879452299757</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0.89229699812925367</v>
+      </c>
+      <c r="M15" s="14">
+        <v>1.2604968981368243</v>
+      </c>
+      <c r="N15" s="21">
+        <v>0.43494800834006392</v>
+      </c>
+      <c r="O15" s="23">
+        <v>7.9562092224762884</v>
+      </c>
+      <c r="P15" s="23">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>7.2304756924160642</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="16" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="14">
+        <v>12.036462028653192</v>
+      </c>
+      <c r="E16" s="14">
+        <v>14.690826870034272</v>
+      </c>
+      <c r="F16" s="14">
+        <v>2.4571173079700253</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4.8604171260649736</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1.8174089333614543</v>
+      </c>
+      <c r="I16" s="14">
+        <v>2.0588000000000002</v>
+      </c>
+      <c r="J16" s="14">
+        <v>2.566584561254897</v>
+      </c>
+      <c r="K16" s="14">
+        <v>1.9537658797263695</v>
+      </c>
+      <c r="L16" s="14">
+        <v>2.1781909222789975</v>
+      </c>
+      <c r="M16" s="14">
+        <v>2.4816289901846873</v>
+      </c>
+      <c r="N16" s="21">
+        <v>4.5037215639801795</v>
+      </c>
+      <c r="O16" s="23">
+        <v>8.1696953402867685</v>
+      </c>
+      <c r="P16" s="23">
+        <v>6.7</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>5.636136560567035</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="14">
+        <v>8.3331494569001308</v>
+      </c>
+      <c r="E17" s="14">
+        <v>3.6874208696079878</v>
+      </c>
+      <c r="F17" s="14">
+        <v>2.2967063175794622</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4.0113695837012733</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.42340246664306652</v>
+      </c>
+      <c r="I17" s="14">
+        <v>1.1879</v>
+      </c>
+      <c r="J17" s="14">
+        <v>0.82824784717641098</v>
+      </c>
+      <c r="K17" s="14">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14">
+        <v>0</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0.88079865305212723</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0</v>
+      </c>
+      <c r="O17" s="23">
+        <v>2.0701729813092102</v>
+      </c>
+      <c r="P17" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>0.28220429532766028</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="14">
+        <v>5.0122940777216947</v>
+      </c>
+      <c r="E18" s="14">
+        <v>8.4390180594440558</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0.9048113995307433</v>
+      </c>
+      <c r="G18" s="14">
+        <v>0</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14">
+        <v>0</v>
+      </c>
+      <c r="K18" s="14">
+        <v>0</v>
+      </c>
+      <c r="L18" s="14">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+      <c r="O18" s="23">
+        <v>2.6482523478927704</v>
+      </c>
+      <c r="P18" s="23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>4.1787877227366739</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3.5353129806100583</v>
+      </c>
+      <c r="E19" s="14">
+        <v>4.8599509512033325</v>
+      </c>
+      <c r="F19" s="14">
+        <v>3.8945633266892905</v>
+      </c>
+      <c r="G19" s="14">
+        <v>2.0810969960991046</v>
+      </c>
+      <c r="H19" s="14">
+        <v>3.1927887343841532</v>
+      </c>
+      <c r="I19" s="14">
+        <v>1.6887000000000001</v>
+      </c>
+      <c r="J19" s="14">
+        <v>3.1263372864926211</v>
+      </c>
+      <c r="K19" s="14">
+        <v>1.6870705087645406</v>
+      </c>
+      <c r="L19" s="14">
+        <v>0.32414908639895251</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0.16260204281171109</v>
+      </c>
+      <c r="N19" s="21">
+        <v>1.3481169038547842</v>
+      </c>
+      <c r="O19" s="23">
+        <v>3.9561647100749857</v>
+      </c>
+      <c r="P19" s="23">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q19" s="23">
+        <v>4.5216072733589767</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.53092532677015958</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1.0193281509036862</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1.1684706283465978</v>
+      </c>
+      <c r="G20" s="14">
+        <v>0.96005330035931602</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0.78439999999999999</v>
+      </c>
+      <c r="J20" s="14">
+        <v>0</v>
+      </c>
+      <c r="K20" s="14">
+        <v>0</v>
+      </c>
+      <c r="L20" s="14">
+        <v>0.32812063618010201</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0.28229127286371936</v>
+      </c>
+      <c r="O20" s="23">
+        <v>9.4645167179465837</v>
+      </c>
+      <c r="P20" s="23">
+        <v>3.9</v>
+      </c>
+      <c r="Q20" s="23">
+        <v>5.6913920534882436</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16">
+        <v>3.5070632421313164</v>
+      </c>
+      <c r="H21" s="16">
+        <v>3.1020289567965551</v>
+      </c>
+      <c r="I21" s="16">
+        <v>1.7009000000000001</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0</v>
+      </c>
+      <c r="K21" s="16">
+        <v>1.1812990540391501</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.55610781362635098</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0</v>
+      </c>
+      <c r="N21" s="22">
+        <v>0</v>
+      </c>
+      <c r="O21" s="24">
+        <v>3.1019579996103404</v>
+      </c>
+      <c r="P21" s="24">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="15">
-        <v>2.4787267316625954</v>
-      </c>
-      <c r="E10" s="15">
-        <v>1.5072935699864518</v>
-      </c>
-      <c r="F10" s="15">
-        <v>0.13114731930321041</v>
-      </c>
-      <c r="G10" s="15">
-        <v>1.9058703261018888</v>
-      </c>
-      <c r="H10" s="15">
-        <v>0</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0.41110000000000002</v>
-      </c>
-      <c r="J10" s="15">
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <v>1.0368879452299757</v>
-      </c>
-      <c r="L10" s="15">
-        <v>0.89229699812925367</v>
-      </c>
-      <c r="M10" s="15">
-        <v>1.2604968981368243</v>
-      </c>
-      <c r="N10" s="22">
-        <v>0.43494800834006392</v>
-      </c>
-      <c r="O10" s="25">
-        <v>7.9562092224762884</v>
-      </c>
-      <c r="P10" s="26">
-        <v>8.8000000000000007</v>
+      <c r="Q21" s="24">
+        <v>1.3988584602956362</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="15">
-        <v>12.036462028653192</v>
-      </c>
-      <c r="E11" s="15">
-        <v>14.690826870034272</v>
-      </c>
-      <c r="F11" s="15">
-        <v>2.4571173079700253</v>
-      </c>
-      <c r="G11" s="15">
-        <v>4.8604171260649736</v>
-      </c>
-      <c r="H11" s="15">
-        <v>1.8174089333614543</v>
-      </c>
-      <c r="I11" s="15">
-        <v>2.0588000000000002</v>
-      </c>
-      <c r="J11" s="15">
-        <v>2.566584561254897</v>
-      </c>
-      <c r="K11" s="15">
-        <v>1.9537658797263695</v>
-      </c>
-      <c r="L11" s="15">
-        <v>2.1781909222789975</v>
-      </c>
-      <c r="M11" s="15">
-        <v>2.4816289901846873</v>
-      </c>
-      <c r="N11" s="22">
-        <v>4.5037215639801795</v>
-      </c>
-      <c r="O11" s="25">
-        <v>8.1696953402867685</v>
-      </c>
-      <c r="P11" s="26">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="15">
-        <v>8.3331494569001308</v>
-      </c>
-      <c r="E12" s="15">
-        <v>3.6874208696079878</v>
-      </c>
-      <c r="F12" s="15">
-        <v>2.2967063175794622</v>
-      </c>
-      <c r="G12" s="15">
-        <v>4.0113695837012733</v>
-      </c>
-      <c r="H12" s="15">
-        <v>0.42340246664306652</v>
-      </c>
-      <c r="I12" s="15">
-        <v>1.1879</v>
-      </c>
-      <c r="J12" s="15">
-        <v>0.82824784717641098</v>
-      </c>
-      <c r="K12" s="15">
-        <v>0</v>
-      </c>
-      <c r="L12" s="15">
-        <v>0</v>
-      </c>
-      <c r="M12" s="15">
-        <v>0.88079865305212723</v>
-      </c>
-      <c r="N12" s="22">
-        <v>0</v>
-      </c>
-      <c r="O12" s="25">
-        <v>2.0701729813092102</v>
-      </c>
-      <c r="P12" s="26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="15">
-        <v>5.0122940777216947</v>
-      </c>
-      <c r="E13" s="15">
-        <v>8.4390180594440558</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0.9048113995307433</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15">
-        <v>0</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15">
-        <v>0</v>
-      </c>
-      <c r="K13" s="15">
-        <v>0</v>
-      </c>
-      <c r="L13" s="15">
-        <v>0</v>
-      </c>
-      <c r="M13" s="15">
-        <v>0</v>
-      </c>
-      <c r="N13" s="22">
-        <v>0</v>
-      </c>
-      <c r="O13" s="25">
-        <v>2.6482523478927704</v>
-      </c>
-      <c r="P13" s="26">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="15">
-        <v>3.5353129806100583</v>
-      </c>
-      <c r="E14" s="15">
-        <v>4.8599509512033325</v>
-      </c>
-      <c r="F14" s="15">
-        <v>3.8945633266892905</v>
-      </c>
-      <c r="G14" s="15">
-        <v>2.0810969960991046</v>
-      </c>
-      <c r="H14" s="15">
-        <v>3.1927887343841532</v>
-      </c>
-      <c r="I14" s="15">
-        <v>1.6887000000000001</v>
-      </c>
-      <c r="J14" s="15">
-        <v>3.1263372864926211</v>
-      </c>
-      <c r="K14" s="15">
-        <v>1.6870705087645406</v>
-      </c>
-      <c r="L14" s="15">
-        <v>0.32414908639895251</v>
-      </c>
-      <c r="M14" s="15">
-        <v>0.16260204281171109</v>
-      </c>
-      <c r="N14" s="22">
-        <v>1.3481169038547842</v>
-      </c>
-      <c r="O14" s="25">
-        <v>3.9561647100749857</v>
-      </c>
-      <c r="P14" s="26">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0.53092532677015958</v>
-      </c>
-      <c r="E15" s="15">
-        <v>1.0193281509036862</v>
-      </c>
-      <c r="F15" s="15">
-        <v>1.1684706283465978</v>
-      </c>
-      <c r="G15" s="15">
-        <v>0.96005330035931602</v>
-      </c>
-      <c r="H15" s="15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15">
-        <v>0.78439999999999999</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="15">
-        <v>0</v>
-      </c>
-      <c r="L15" s="15">
-        <v>0.32812063618010201</v>
-      </c>
-      <c r="M15" s="15">
-        <v>0</v>
-      </c>
-      <c r="N15" s="22">
-        <v>0.28229127286371936</v>
-      </c>
-      <c r="O15" s="25">
-        <v>9.4645167179465837</v>
-      </c>
-      <c r="P15" s="26">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="12.75" thickBot="1">
-      <c r="A16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="10" t="s">
+    <row r="22" spans="1:17" s="9" customFormat="1">
+      <c r="A22" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="17">
-        <v>3.5070632421313164</v>
-      </c>
-      <c r="H16" s="17">
-        <v>3.1020289567965551</v>
-      </c>
-      <c r="I16" s="17">
-        <v>1.7009000000000001</v>
-      </c>
-      <c r="J16" s="17">
-        <v>0</v>
-      </c>
-      <c r="K16" s="17">
-        <v>1.1812990540391501</v>
-      </c>
-      <c r="L16" s="17">
-        <v>0.55610781362635098</v>
-      </c>
-      <c r="M16" s="17">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
-        <v>0</v>
-      </c>
-      <c r="O16" s="27">
-        <v>3.1019579996103404</v>
-      </c>
-      <c r="P16" s="27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="9" customFormat="1">
-      <c r="A17" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>20</v>
+      <c r="C22" s="25" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>